<commit_message>
2017-06-01 / SHA256 of zip AAC108610B6D090333798D4CAEC262BBD4EE277D5D727BC97CBAB01C56E94F13
</commit_message>
<xml_diff>
--- a/Extras/PowerShell_and_Python.xlsx
+++ b/Extras/PowerShell_and_Python.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SANS\CD-ROM\Root-NEW\Day1-PowerShell\Misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SANS\USB\Root\Extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="3105" windowWidth="18195" windowHeight="12345"/>
+    <workbookView xWindow="480" yWindow="4305" windowWidth="18195" windowHeight="12345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="262">
   <si>
     <t>Object oriented</t>
   </si>
@@ -730,12 +730,6 @@
     <t>Use .NET timer explicitly, and Measure-Command.</t>
   </si>
   <si>
-    <t xml:space="preserve">     Various Google trends reports (www.google.com/trends) from Nov 2006 to Feb 2016:</t>
-  </si>
-  <si>
-    <t>The following RedMonk/HP chart from http://redmonk.com/sogrady/2016/02/19/language-rankings-1-16/</t>
-  </si>
-  <si>
     <t>Create private variables and methods</t>
   </si>
   <si>
@@ -803,6 +797,15 @@
   </si>
   <si>
     <t>https://github.com/dlwyatt/PowershellProfiler</t>
+  </si>
+  <si>
+    <t>The following RedMonk/HP chart from http://redmonk.com/sogrady/2017/03/17/language-rankings-1-17/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Various Google trends reports (www.google.com/trends) from Nov 2006 to May 2017:</t>
+  </si>
+  <si>
+    <t>Title: Python or PowerShell (see below)</t>
   </si>
 </sst>
 </file>
@@ -967,7 +970,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1007,6 +1010,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1049,7 +1053,7 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4368568" cy="4961615"/>
@@ -1390,19 +1394,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>73187</xdr:rowOff>
+      <xdr:colOff>385906</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1415,8 +1419,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="685800" y="6581775"/>
-          <a:ext cx="8258175" cy="5731037"/>
+          <a:off x="714375" y="1123951"/>
+          <a:ext cx="8339281" cy="4438650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1428,19 +1432,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>253514</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>110408</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1453,8 +1457,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="714375" y="885825"/>
-          <a:ext cx="8206889" cy="5619749"/>
+          <a:off x="742950" y="5981701"/>
+          <a:ext cx="8334375" cy="4463332"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1466,19 +1470,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>268168</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>185458</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPr id="5" name="Picture 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1491,8 +1495,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="695325" y="12487275"/>
-          <a:ext cx="8240593" cy="5657849"/>
+          <a:off x="771525" y="10848975"/>
+          <a:ext cx="8296275" cy="4433608"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1504,19 +1508,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>130</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>233362</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>130968</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>169</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>583514</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPr id="11" name="Picture 10"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1536,8 +1540,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="38100" y="25069800"/>
-          <a:ext cx="10972800" cy="7324725"/>
+          <a:off x="233362" y="23371968"/>
+          <a:ext cx="10208527" cy="7503319"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1554,6 +1558,96 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2628900" y="31022926"/>
+          <a:ext cx="6038850" cy="1885950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Quote from the above RedMonk</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> article (March 2017):</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>"PowerShell: As mentioned above, no top tier language outperformed TypeScript on the GitHub portion of our rankings, but one language equaled it. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>PowerShell moved from 36 within the GitHub rankings to 19 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>to match TypeScript’s 17 point jump, and that was enough to nudge it into the Top 20 overall from its prior ranking of 25. While we can’t prove causation, it is interesting to note that this dramatic improvement from PowerShell comes one quarter after it was released as open source software. Between PowerShell and TypeScript, not to mention C#’s sustained performance, Microsoft has reason to be pleased about is programming language investments."</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1848,18 +1942,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.875" customWidth="1"/>
-    <col min="2" max="2" width="42.25" customWidth="1"/>
-    <col min="3" max="3" width="13.75" customWidth="1"/>
-    <col min="4" max="4" width="11.25" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="66" customWidth="1"/>
-    <col min="6" max="6" width="46.625" customWidth="1"/>
+    <col min="6" max="6" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
@@ -1874,7 +1968,7 @@
     </row>
     <row r="3" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1918,7 +2012,7 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1952,7 +2046,7 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1969,7 +2063,7 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2025,7 +2119,7 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>5</v>
@@ -2097,7 +2191,7 @@
         <v>161</v>
       </c>
       <c r="B20" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>3</v>
@@ -2262,7 +2356,7 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2279,7 +2373,7 @@
         <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F31" t="s">
         <v>34</v>
@@ -2573,10 +2667,10 @@
         <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2627,7 +2721,7 @@
         <v>3</v>
       </c>
       <c r="E53" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2658,7 +2752,7 @@
         <v>5</v>
       </c>
       <c r="E55" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F55" t="s">
         <v>154</v>
@@ -2678,7 +2772,7 @@
         <v>3</v>
       </c>
       <c r="E56" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F56" t="s">
         <v>129</v>
@@ -2720,7 +2814,7 @@
         <v>54</v>
       </c>
       <c r="B59" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C59" t="s">
         <v>3</v>
@@ -3012,7 +3106,7 @@
         <v>36</v>
       </c>
       <c r="B78" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>3</v>
@@ -3026,7 +3120,7 @@
         <v>36</v>
       </c>
       <c r="B79" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C79" s="18" t="s">
         <v>5</v>
@@ -3035,10 +3129,10 @@
         <v>3</v>
       </c>
       <c r="E79" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F79" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -3046,7 +3140,7 @@
         <v>36</v>
       </c>
       <c r="B80" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C80" s="18" t="s">
         <v>5</v>
@@ -3055,7 +3149,7 @@
         <v>3</v>
       </c>
       <c r="F80" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -3546,7 +3640,7 @@
         <v>3</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F113" s="6" t="s">
         <v>230</v>
@@ -3606,7 +3700,7 @@
         <v>3</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F116" s="6" t="s">
         <v>231</v>
@@ -3801,12 +3895,12 @@
         <v>191</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3828,20 +3922,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P173"/>
+  <dimension ref="B2:P164"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="15"/>
-    <col min="2" max="2" width="11.375" style="15" customWidth="1"/>
-    <col min="3" max="3" width="13.875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="9.125" style="15"/>
-    <col min="5" max="5" width="13.25" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.125" style="15"/>
+    <col min="1" max="1" width="9.140625" style="15"/>
+    <col min="2" max="2" width="11.42578125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="15"/>
+    <col min="5" max="5" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
@@ -3863,7 +3957,7 @@
     </row>
     <row r="3" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -3897,81 +3991,234 @@
       <c r="O4" s="22"/>
       <c r="P4" s="22"/>
     </row>
-    <row r="100" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B100" s="16" t="s">
+    <row r="86" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B86" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="C100" s="22"/>
-      <c r="D100" s="22"/>
-      <c r="E100" s="22"/>
-      <c r="F100" s="22"/>
-      <c r="G100" s="22"/>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B101" s="26" t="s">
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="22"/>
+      <c r="G86" s="22"/>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="C101" s="24" t="s">
+      <c r="C87" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="D101" s="24"/>
-      <c r="E101" s="24" t="s">
+      <c r="D87" s="24"/>
+      <c r="E87" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="F101" s="24"/>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F87" s="24"/>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="30">
+        <v>42220</v>
+      </c>
+      <c r="C88" s="29">
+        <v>649000</v>
+      </c>
+      <c r="D88" s="29"/>
+      <c r="E88" s="29">
+        <v>525000</v>
+      </c>
+      <c r="F88" s="25"/>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="30">
+        <v>42319</v>
+      </c>
+      <c r="C89" s="29">
+        <v>698000</v>
+      </c>
+      <c r="D89" s="29"/>
+      <c r="E89" s="29">
+        <v>507000</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="30">
+        <v>42425</v>
+      </c>
+      <c r="C90" s="29">
+        <v>384000</v>
+      </c>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29">
+        <v>535000</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="30">
+        <v>42564</v>
+      </c>
+      <c r="C91" s="28">
+        <v>461000</v>
+      </c>
+      <c r="D91" s="28"/>
+      <c r="E91" s="28">
+        <v>475000</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="30">
+        <v>42728</v>
+      </c>
+      <c r="C92" s="28">
+        <v>543000</v>
+      </c>
+      <c r="D92" s="28"/>
+      <c r="E92" s="28">
+        <v>527000</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="30">
+        <v>42865</v>
+      </c>
+      <c r="C93" s="28">
+        <v>605000</v>
+      </c>
+      <c r="D93" s="28"/>
+      <c r="E93" s="28">
+        <v>529000</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B95" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="C95" s="22"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="22"/>
+      <c r="F95" s="22"/>
+      <c r="G95" s="22"/>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="C96" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="D96" s="24"/>
+      <c r="E96" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="F96" s="24"/>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="30">
+        <v>42220</v>
+      </c>
+      <c r="C97" s="29">
+        <v>840000</v>
+      </c>
+      <c r="D97" s="29"/>
+      <c r="E97" s="29">
+        <v>1210000</v>
+      </c>
+      <c r="F97" s="25"/>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="30">
+        <v>42319</v>
+      </c>
+      <c r="C98" s="29">
+        <v>776000</v>
+      </c>
+      <c r="D98" s="29"/>
+      <c r="E98" s="29">
+        <v>1610000</v>
+      </c>
+      <c r="F98" s="25"/>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="30">
+        <v>42425</v>
+      </c>
+      <c r="C99" s="29">
+        <v>890000</v>
+      </c>
+      <c r="D99" s="29"/>
+      <c r="E99" s="29">
+        <v>1240000</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="30">
+        <v>42564</v>
+      </c>
+      <c r="C100" s="28">
+        <v>1310000</v>
+      </c>
+      <c r="D100" s="28"/>
+      <c r="E100" s="28">
+        <v>1950000</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="30">
+        <v>42728</v>
+      </c>
+      <c r="C101" s="28">
+        <v>684000</v>
+      </c>
+      <c r="D101" s="28"/>
+      <c r="E101" s="28">
+        <v>1060000</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102" s="30">
-        <v>42220</v>
-      </c>
-      <c r="C102" s="29">
-        <v>649000</v>
-      </c>
-      <c r="D102" s="29"/>
-      <c r="E102" s="29">
-        <v>525000</v>
-      </c>
-      <c r="F102" s="25"/>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B103" s="30">
-        <v>42319</v>
-      </c>
-      <c r="C103" s="29">
-        <v>698000</v>
-      </c>
-      <c r="D103" s="29"/>
-      <c r="E103" s="29">
-        <v>507000</v>
-      </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B104" s="30">
-        <v>42425</v>
-      </c>
-      <c r="C104" s="29">
-        <v>384000</v>
-      </c>
-      <c r="D104" s="29"/>
-      <c r="E104" s="29">
-        <v>535000</v>
-      </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B105" s="30">
-        <v>42564</v>
-      </c>
-      <c r="C105" s="28">
-        <v>461000</v>
-      </c>
-      <c r="D105" s="28"/>
-      <c r="E105" s="28">
-        <v>475000</v>
-      </c>
-    </row>
-    <row r="107" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B107" s="16" t="s">
-        <v>216</v>
+        <v>42865</v>
+      </c>
+      <c r="C102" s="28">
+        <v>715000</v>
+      </c>
+      <c r="D102" s="28"/>
+      <c r="E102" s="28">
+        <v>888000</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B104" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="C104" s="22"/>
+      <c r="D104" s="22"/>
+      <c r="E104" s="22"/>
+      <c r="F104" s="22"/>
+      <c r="G104" s="22"/>
+      <c r="H104" s="23"/>
+    </row>
+    <row r="105" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B105" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="C105" s="22"/>
+      <c r="D105" s="22"/>
+      <c r="E105" s="22"/>
+      <c r="F105" s="22"/>
+      <c r="G105" s="22"/>
+      <c r="H105" s="23"/>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B106" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="C106" s="22"/>
+      <c r="D106" s="22"/>
+      <c r="E106" s="22"/>
+      <c r="F106" s="22"/>
+      <c r="G106" s="22"/>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B107" s="22" t="s">
+        <v>225</v>
       </c>
       <c r="C107" s="22"/>
       <c r="D107" s="22"/>
@@ -3979,217 +4226,145 @@
       <c r="F107" s="22"/>
       <c r="G107" s="22"/>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B108" s="26" t="s">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B108" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="C108" s="22"/>
+      <c r="D108" s="22"/>
+      <c r="E108" s="22"/>
+      <c r="F108" s="22"/>
+      <c r="G108" s="22"/>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B109" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="C109" s="22"/>
+      <c r="D109" s="22"/>
+      <c r="E109" s="22"/>
+      <c r="F109" s="22"/>
+      <c r="G109" s="22"/>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B110" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C110" s="22"/>
+      <c r="D110" s="22"/>
+      <c r="E110" s="22"/>
+      <c r="F110" s="22"/>
+      <c r="G110" s="22"/>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B111" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="C111" s="22"/>
+      <c r="D111" s="22"/>
+      <c r="E111" s="22"/>
+      <c r="F111" s="22"/>
+      <c r="G111" s="22"/>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B112" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="C108" s="24" t="s">
-        <v>213</v>
-      </c>
-      <c r="D108" s="24"/>
-      <c r="E108" s="24" t="s">
-        <v>214</v>
-      </c>
-      <c r="F108" s="24"/>
-    </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B109" s="30">
+      <c r="C112" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="D112" s="24"/>
+      <c r="E112" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="F112" s="24"/>
+    </row>
+    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B113" s="30">
         <v>42220</v>
       </c>
-      <c r="C109" s="29">
-        <v>840000</v>
-      </c>
-      <c r="D109" s="29"/>
-      <c r="E109" s="29">
-        <v>1210000</v>
-      </c>
-      <c r="F109" s="25"/>
-    </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B110" s="30">
+      <c r="C113" s="25">
+        <v>484</v>
+      </c>
+      <c r="D113" s="25"/>
+      <c r="E113" s="25">
+        <v>119</v>
+      </c>
+      <c r="F113" s="25"/>
+    </row>
+    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B114" s="30">
         <v>42319</v>
       </c>
-      <c r="C110" s="29">
-        <v>776000</v>
-      </c>
-      <c r="D110" s="29"/>
-      <c r="E110" s="29">
-        <v>1610000</v>
-      </c>
-      <c r="F110" s="25"/>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B111" s="30">
+      <c r="C114" s="25">
+        <v>653</v>
+      </c>
+      <c r="D114" s="25"/>
+      <c r="E114" s="25">
+        <v>142</v>
+      </c>
+      <c r="F114" s="25"/>
+    </row>
+    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B115" s="30">
         <v>42425</v>
       </c>
-      <c r="C111" s="29">
-        <v>890000</v>
-      </c>
-      <c r="D111" s="29"/>
-      <c r="E111" s="29">
-        <v>1240000</v>
-      </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B112" s="30">
+      <c r="C115" s="15">
+        <v>701</v>
+      </c>
+      <c r="E115" s="15">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B116" s="30">
         <v>42564</v>
       </c>
-      <c r="C112" s="28">
-        <v>1310000</v>
-      </c>
-      <c r="D112" s="28"/>
-      <c r="E112" s="28">
-        <v>1950000</v>
-      </c>
-    </row>
-    <row r="114" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B114" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="C114" s="22"/>
-      <c r="D114" s="22"/>
-      <c r="E114" s="22"/>
-      <c r="F114" s="22"/>
-      <c r="G114" s="22"/>
-      <c r="H114" s="23"/>
-    </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B115" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C115" s="22"/>
-      <c r="D115" s="22"/>
-      <c r="E115" s="22"/>
-      <c r="F115" s="22"/>
-      <c r="G115" s="22"/>
-    </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B116" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="C116" s="22"/>
-      <c r="D116" s="22"/>
-      <c r="E116" s="22"/>
-      <c r="F116" s="22"/>
-      <c r="G116" s="22"/>
-    </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B117" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="C117" s="22"/>
-      <c r="D117" s="22"/>
-      <c r="E117" s="22"/>
-      <c r="F117" s="22"/>
-      <c r="G117" s="22"/>
-    </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B118" s="22" t="s">
-        <v>223</v>
-      </c>
-      <c r="C118" s="22"/>
-      <c r="D118" s="22"/>
-      <c r="E118" s="22"/>
-      <c r="F118" s="22"/>
-      <c r="G118" s="22"/>
-    </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B119" s="22" t="s">
-        <v>221</v>
-      </c>
-      <c r="C119" s="22"/>
-      <c r="D119" s="22"/>
-      <c r="E119" s="22"/>
-      <c r="F119" s="22"/>
-      <c r="G119" s="22"/>
-    </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B120" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="C120" s="22"/>
-      <c r="D120" s="22"/>
-      <c r="E120" s="22"/>
-      <c r="F120" s="22"/>
-      <c r="G120" s="22"/>
-    </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B121" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="C121" s="24" t="s">
-        <v>218</v>
-      </c>
-      <c r="D121" s="24"/>
-      <c r="E121" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="F121" s="24"/>
-    </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B122" s="30">
-        <v>42220</v>
-      </c>
-      <c r="C122" s="25">
-        <v>484</v>
-      </c>
-      <c r="D122" s="25"/>
-      <c r="E122" s="25">
-        <v>119</v>
-      </c>
-      <c r="F122" s="25"/>
-    </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B123" s="30">
-        <v>42319</v>
-      </c>
-      <c r="C123" s="25">
-        <v>653</v>
-      </c>
-      <c r="D123" s="25"/>
-      <c r="E123" s="25">
-        <v>142</v>
-      </c>
-      <c r="F123" s="25"/>
-    </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B124" s="30">
-        <v>42425</v>
-      </c>
-      <c r="C124" s="15">
-        <v>701</v>
-      </c>
-      <c r="E124" s="15">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B125" s="30">
-        <v>42564</v>
-      </c>
-      <c r="C125" s="15">
+      <c r="C116" s="15">
         <v>759</v>
       </c>
-      <c r="E125" s="15">
+      <c r="E116" s="15">
         <v>172</v>
       </c>
     </row>
-    <row r="130" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B130" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="C130" s="22"/>
-      <c r="D130" s="22"/>
-      <c r="E130" s="22"/>
-      <c r="F130" s="22"/>
-      <c r="G130" s="22"/>
-      <c r="H130" s="22"/>
-      <c r="I130" s="22"/>
-      <c r="J130" s="22"/>
-      <c r="K130" s="22"/>
-    </row>
-    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C173"/>
+    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B117" s="31">
+        <v>42728</v>
+      </c>
+      <c r="C117" s="15">
+        <v>870</v>
+      </c>
+      <c r="E117" s="15">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B118" s="31">
+        <v>42865</v>
+      </c>
+      <c r="C118" s="15">
+        <v>1023</v>
+      </c>
+      <c r="E118" s="15">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="121" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B121" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="C121" s="22"/>
+      <c r="D121" s="22"/>
+      <c r="E121" s="22"/>
+      <c r="F121" s="22"/>
+      <c r="G121" s="22"/>
+      <c r="H121" s="22"/>
+      <c r="I121" s="22"/>
+      <c r="J121" s="22"/>
+      <c r="K121" s="22"/>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C164"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2018-02-06T19:06:11 / SHA256 of zip 51AEBB2B92FFABD03137D0CB61389629E97BB74356D5E4D841D8FD539CF96F1F
</commit_message>
<xml_diff>
--- a/Extras/PowerShell_and_Python.xlsx
+++ b/Extras/PowerShell_and_Python.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="4305" windowWidth="18195" windowHeight="12345" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="4905" windowWidth="18195" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -799,13 +799,13 @@
     <t>https://github.com/dlwyatt/PowershellProfiler</t>
   </si>
   <si>
-    <t>The following RedMonk/HP chart from http://redmonk.com/sogrady/2017/03/17/language-rankings-1-17/</t>
-  </si>
-  <si>
     <t xml:space="preserve">     Various Google trends reports (www.google.com/trends) from Nov 2006 to May 2017:</t>
   </si>
   <si>
     <t>Title: Python or PowerShell (see below)</t>
+  </si>
+  <si>
+    <t>The following RedMonk/HP chart from https://redmonk.com/sogrady/2017/06/08/language-rankings-6-17/</t>
   </si>
 </sst>
 </file>
@@ -1508,19 +1508,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>233362</xdr:colOff>
-      <xdr:row>122</xdr:row>
-      <xdr:rowOff>130968</xdr:rowOff>
+      <xdr:colOff>52916</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>159210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>583514</xdr:colOff>
-      <xdr:row>162</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:colOff>201083</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>134408</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPr id="8" name="Picture 7"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1540,8 +1540,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="233362" y="23371968"/>
-          <a:ext cx="10208527" cy="7503319"/>
+          <a:off x="52916" y="23474293"/>
+          <a:ext cx="10085917" cy="6452198"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1558,96 +1558,6 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>162</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>172</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2628900" y="31022926"/>
-          <a:ext cx="6038850" cy="1885950"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Quote from the above RedMonk</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> article (March 2017):</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>"PowerShell: As mentioned above, no top tier language outperformed TypeScript on the GitHub portion of our rankings, but one language equaled it. </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>PowerShell moved from 36 within the GitHub rankings to 19 </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>to match TypeScript’s 17 point jump, and that was enough to nudge it into the Top 20 overall from its prior ranking of 25. While we can’t prove causation, it is interesting to note that this dramatic improvement from PowerShell comes one quarter after it was released as open source software. Between PowerShell and TypeScript, not to mention C#’s sustained performance, Microsoft has reason to be pleased about is programming language investments."</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1942,8 +1852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A130" sqref="A130"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3924,8 +3834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3957,7 +3867,7 @@
     </row>
     <row r="3" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -4197,7 +4107,7 @@
     </row>
     <row r="105" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B105" s="22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C105" s="22"/>
       <c r="D105" s="22"/>
@@ -4351,7 +4261,7 @@
     </row>
     <row r="121" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B121" s="27" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C121" s="22"/>
       <c r="D121" s="22"/>

</xml_diff>